<commit_message>
AI-refactor four type contoursCalc alogrithm
</commit_message>
<xml_diff>
--- a/z-tools/test/image_basic_feature/contoursCalc/Args.xlsx
+++ b/z-tools/test/image_basic_feature/contoursCalc/Args.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="20190122_2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="20190119" sheetId="5" r:id="rId1"/>
+    <sheet name="20190122_1" sheetId="4" r:id="rId2"/>
+    <sheet name="20190122_2" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="16">
   <si>
     <t>H</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -226,12 +226,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -240,15 +234,21 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -550,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -562,86 +562,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16.2" x14ac:dyDescent="0.4">
-      <c r="A1" s="7"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="3" t="s">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="7"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" ht="16.2" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="H2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="9" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="9" t="s">
+      <c r="Q2" s="11"/>
+      <c r="R2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="8" t="s">
+      <c r="S2" s="11"/>
+      <c r="T2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -653,10 +653,10 @@
       <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
         <v>0.04</v>
       </c>
       <c r="E3" s="2">
@@ -674,10 +674,10 @@
       <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="I3" s="6">
-        <v>1</v>
-      </c>
-      <c r="J3" s="11">
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
         <v>0.1</v>
       </c>
       <c r="K3" s="2">
@@ -716,7 +716,1731 @@
         <f>M3</f>
         <v>25.5</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="T3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <f t="shared" ref="A4:A17" si="0">ROW()-2</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E17" si="1">B4/2</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:G17" si="2">C4*255</f>
+        <v>255</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="2"/>
+        <v>12.75</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K17" si="3">H4/2</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:M17" si="4">I4*255</f>
+        <v>255</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="4"/>
+        <v>45.9</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N17" si="5">E4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O17" si="6">K4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P17" si="7">F4</f>
+        <v>255</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" ref="Q4:Q17" si="8">L4</f>
+        <v>255</v>
+      </c>
+      <c r="R4" s="2">
+        <f t="shared" ref="R4:R17" si="9">G4</f>
+        <v>12.75</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" ref="S4:S17" si="10">M4</f>
+        <v>45.9</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="2"/>
+        <v>15.299999999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="4"/>
+        <v>33.15</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R5" s="2">
+        <f t="shared" si="9"/>
+        <v>15.299999999999999</v>
+      </c>
+      <c r="S5" s="2">
+        <f t="shared" si="10"/>
+        <v>33.15</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="4"/>
+        <v>48.45</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R6" s="2">
+        <f t="shared" si="9"/>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" si="10"/>
+        <v>48.45</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="4"/>
+        <v>127.5</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" si="9"/>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="10"/>
+        <v>127.5</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.43</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="4"/>
+        <v>109.64999999999999</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="9"/>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="10"/>
+        <v>109.64999999999999</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.36</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>91.8</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.44</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="4"/>
+        <v>112.2</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="9"/>
+        <v>91.8</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="10"/>
+        <v>112.2</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>20.400000000000002</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="4"/>
+        <v>127.5</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="9"/>
+        <v>20.400000000000002</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="10"/>
+        <v>127.5</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="4"/>
+        <v>33.15</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="9"/>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="10"/>
+        <v>33.15</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="4"/>
+        <v>28.05</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="9"/>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="10"/>
+        <v>28.05</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="2"/>
+        <v>25.5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="4"/>
+        <v>102</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="9"/>
+        <v>25.5</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="10"/>
+        <v>102</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>61.199999999999996</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="4"/>
+        <v>229.5</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="9"/>
+        <v>61.199999999999996</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="10"/>
+        <v>229.5</v>
+      </c>
+      <c r="T14" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="2"/>
+        <v>33.15</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="4"/>
+        <v>127.5</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" si="9"/>
+        <v>33.15</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="10"/>
+        <v>127.5</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="4"/>
+        <v>104.55</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="9"/>
+        <v>102</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="10"/>
+        <v>104.55</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="4"/>
+        <v>104.55</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="9"/>
+        <v>102</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="10"/>
+        <v>104.55</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="16.2" x14ac:dyDescent="0.4">
+      <c r="A1" s="5"/>
+      <c r="B1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" ht="16.2" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="11"/>
+      <c r="T2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <f>ROW()-2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="E3" s="2">
+        <f>B3/2</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <f>C3*255</f>
+        <v>255</v>
+      </c>
+      <c r="G3" s="2">
+        <f>D3*255</f>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="2">
+        <f>H3/2</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <f>I3*255</f>
+        <v>255</v>
+      </c>
+      <c r="M3" s="2">
+        <f>J3*255</f>
+        <v>25.5</v>
+      </c>
+      <c r="N3" s="2">
+        <f>E3</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <f>K3</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <f>F3</f>
+        <v>255</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>L3</f>
+        <v>255</v>
+      </c>
+      <c r="R3" s="2">
+        <f>G3</f>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="S3" s="2">
+        <f>M3</f>
+        <v>25.5</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <f t="shared" ref="A4:A7" si="0">ROW()-2</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E7" si="1">B4/2</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:G7" si="2">C4*255</f>
+        <v>255</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="2"/>
+        <v>12.75</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K7" si="3">H4/2</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:M7" si="4">I4*255</f>
+        <v>255</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="4"/>
+        <v>45.9</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N7" si="5">E4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O7" si="6">K4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P7" si="7">F4</f>
+        <v>255</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" ref="Q4:Q7" si="8">L4</f>
+        <v>255</v>
+      </c>
+      <c r="R4" s="2">
+        <f t="shared" ref="R4:R7" si="9">G4</f>
+        <v>12.75</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" ref="S4:S7" si="10">M4</f>
+        <v>45.9</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="2"/>
+        <v>15.299999999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="4"/>
+        <v>33.15</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R5" s="2">
+        <f t="shared" si="9"/>
+        <v>15.299999999999999</v>
+      </c>
+      <c r="S5" s="2">
+        <f t="shared" si="10"/>
+        <v>33.15</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="4"/>
+        <v>48.45</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R6" s="2">
+        <f t="shared" si="9"/>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" si="10"/>
+        <v>48.45</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="4"/>
+        <v>127.5</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="8"/>
+        <v>255</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" si="9"/>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="10"/>
+        <v>127.5</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="16.2" x14ac:dyDescent="0.4">
+      <c r="A1" s="5"/>
+      <c r="B1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" ht="16.2" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="11"/>
+      <c r="T2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <f>ROW()-2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="E3" s="2">
+        <f>B3/2</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <f>C3*255</f>
+        <v>255</v>
+      </c>
+      <c r="G3" s="2">
+        <f>D3*255</f>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="2">
+        <f>H3/2</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <f>I3*255</f>
+        <v>255</v>
+      </c>
+      <c r="M3" s="2">
+        <f>J3*255</f>
+        <v>25.5</v>
+      </c>
+      <c r="N3" s="2">
+        <f>E3</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <f>K3</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <f>F3</f>
+        <v>255</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>L3</f>
+        <v>255</v>
+      </c>
+      <c r="R3" s="2">
+        <f>G3</f>
+        <v>10.200000000000001</v>
+      </c>
+      <c r="S3" s="2">
+        <f>M3</f>
+        <v>25.5</v>
+      </c>
+      <c r="T3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -728,10 +2452,10 @@
       <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
         <v>0.05</v>
       </c>
       <c r="E4" s="2">
@@ -749,10 +2473,10 @@
       <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="I4" s="6">
-        <v>1</v>
-      </c>
-      <c r="J4" s="11">
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
         <v>0.18</v>
       </c>
       <c r="K4" s="2">
@@ -791,7 +2515,7 @@
         <f t="shared" ref="S4:S20" si="12">M4</f>
         <v>45.9</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="T4" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -803,10 +2527,10 @@
       <c r="B5" s="2">
         <v>0</v>
       </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
         <v>0.06</v>
       </c>
       <c r="E5" s="2">
@@ -824,10 +2548,10 @@
       <c r="H5" s="2">
         <v>0</v>
       </c>
-      <c r="I5" s="6">
-        <v>1</v>
-      </c>
-      <c r="J5" s="11">
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
         <v>0.13</v>
       </c>
       <c r="K5" s="2">
@@ -866,7 +2590,7 @@
         <f t="shared" si="12"/>
         <v>33.15</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="T5" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -878,10 +2602,10 @@
       <c r="B6" s="2">
         <v>0</v>
       </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11">
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
         <v>0.04</v>
       </c>
       <c r="E6" s="2">
@@ -899,10 +2623,10 @@
       <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="I6" s="6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="11">
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
         <v>0.19</v>
       </c>
       <c r="K6" s="2">
@@ -941,7 +2665,7 @@
         <f t="shared" si="12"/>
         <v>48.45</v>
       </c>
-      <c r="T6" s="13" t="s">
+      <c r="T6" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -953,10 +2677,10 @@
       <c r="B7" s="2">
         <v>0</v>
       </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
         <v>0.14000000000000001</v>
       </c>
       <c r="E7" s="2">
@@ -974,10 +2698,10 @@
       <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7" s="6">
-        <v>1</v>
-      </c>
-      <c r="J7" s="11">
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
         <v>0.5</v>
       </c>
       <c r="K7" s="2">
@@ -1016,7 +2740,7 @@
         <f t="shared" si="12"/>
         <v>127.5</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="T7" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1028,10 +2752,10 @@
       <c r="B8" s="2">
         <v>0</v>
       </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
         <v>0.14000000000000001</v>
       </c>
       <c r="E8" s="2">
@@ -1049,10 +2773,10 @@
       <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
         <v>0.43</v>
       </c>
       <c r="K8" s="2">
@@ -1091,7 +2815,7 @@
         <f t="shared" si="12"/>
         <v>109.64999999999999</v>
       </c>
-      <c r="T8" s="13" t="s">
+      <c r="T8" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1103,10 +2827,10 @@
       <c r="B9" s="2">
         <v>0</v>
       </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
         <v>0.36</v>
       </c>
       <c r="E9" s="2">
@@ -1124,10 +2848,10 @@
       <c r="H9" s="2">
         <v>0</v>
       </c>
-      <c r="I9" s="6">
-        <v>1</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7">
         <v>0.44</v>
       </c>
       <c r="K9" s="2">
@@ -1166,7 +2890,7 @@
         <f t="shared" si="12"/>
         <v>112.2</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="T9" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1178,10 +2902,10 @@
       <c r="B10" s="2">
         <v>0</v>
       </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11">
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
         <v>0.08</v>
       </c>
       <c r="E10" s="2">
@@ -1199,10 +2923,10 @@
       <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="6">
-        <v>1</v>
-      </c>
-      <c r="J10" s="11">
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7">
         <v>0.5</v>
       </c>
       <c r="K10" s="2">
@@ -1241,7 +2965,7 @@
         <f t="shared" si="12"/>
         <v>127.5</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="T10" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1253,10 +2977,10 @@
       <c r="B11" s="2">
         <v>0</v>
       </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11">
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
         <v>0.04</v>
       </c>
       <c r="E11" s="2">
@@ -1274,10 +2998,10 @@
       <c r="H11" s="2">
         <v>0</v>
       </c>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-      <c r="J11" s="11">
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
         <v>0.13</v>
       </c>
       <c r="K11" s="2">
@@ -1316,7 +3040,7 @@
         <f t="shared" si="12"/>
         <v>33.15</v>
       </c>
-      <c r="T11" s="13" t="s">
+      <c r="T11" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1328,10 +3052,10 @@
       <c r="B12" s="2">
         <v>0</v>
       </c>
-      <c r="C12" s="6">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11">
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
         <v>0.04</v>
       </c>
       <c r="E12" s="2">
@@ -1349,10 +3073,10 @@
       <c r="H12" s="2">
         <v>0</v>
       </c>
-      <c r="I12" s="6">
-        <v>1</v>
-      </c>
-      <c r="J12" s="11">
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
         <v>0.11</v>
       </c>
       <c r="K12" s="2">
@@ -1391,7 +3115,7 @@
         <f t="shared" si="12"/>
         <v>28.05</v>
       </c>
-      <c r="T12" s="13" t="s">
+      <c r="T12" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1403,10 +3127,10 @@
       <c r="B13" s="2">
         <v>0</v>
       </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13" s="11">
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
         <v>0.1</v>
       </c>
       <c r="E13" s="2">
@@ -1424,10 +3148,10 @@
       <c r="H13" s="2">
         <v>0</v>
       </c>
-      <c r="I13" s="6">
-        <v>1</v>
-      </c>
-      <c r="J13" s="11">
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7">
         <v>0.4</v>
       </c>
       <c r="K13" s="2">
@@ -1466,7 +3190,7 @@
         <f t="shared" si="12"/>
         <v>102</v>
       </c>
-      <c r="T13" s="13" t="s">
+      <c r="T13" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1478,10 +3202,10 @@
       <c r="B14" s="2">
         <v>0</v>
       </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11">
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
         <v>0.24</v>
       </c>
       <c r="E14" s="2">
@@ -1499,10 +3223,10 @@
       <c r="H14" s="2">
         <v>0</v>
       </c>
-      <c r="I14" s="6">
-        <v>1</v>
-      </c>
-      <c r="J14" s="11">
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7">
         <v>0.9</v>
       </c>
       <c r="K14" s="2">
@@ -1541,7 +3265,7 @@
         <f t="shared" si="12"/>
         <v>229.5</v>
       </c>
-      <c r="T14" s="13" t="s">
+      <c r="T14" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1553,10 +3277,10 @@
       <c r="B15" s="2">
         <v>0</v>
       </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-      <c r="D15" s="11">
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
         <v>0.13</v>
       </c>
       <c r="E15" s="2">
@@ -1574,10 +3298,10 @@
       <c r="H15" s="2">
         <v>0</v>
       </c>
-      <c r="I15" s="6">
-        <v>1</v>
-      </c>
-      <c r="J15" s="11">
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7">
         <v>0.5</v>
       </c>
       <c r="K15" s="2">
@@ -1616,7 +3340,7 @@
         <f t="shared" si="12"/>
         <v>127.5</v>
       </c>
-      <c r="T15" s="13" t="s">
+      <c r="T15" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1628,10 +3352,10 @@
       <c r="B16" s="2">
         <v>0</v>
       </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16" s="11">
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
         <v>0.4</v>
       </c>
       <c r="E16" s="2">
@@ -1649,10 +3373,10 @@
       <c r="H16" s="2">
         <v>0</v>
       </c>
-      <c r="I16" s="6">
-        <v>1</v>
-      </c>
-      <c r="J16" s="11">
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
         <v>0.41</v>
       </c>
       <c r="K16" s="2">
@@ -1691,7 +3415,7 @@
         <f t="shared" si="12"/>
         <v>104.55</v>
       </c>
-      <c r="T16" s="13" t="s">
+      <c r="T16" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1703,10 +3427,10 @@
       <c r="B17" s="2">
         <v>0</v>
       </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17" s="11">
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
         <v>0.4</v>
       </c>
       <c r="E17" s="2">
@@ -1724,10 +3448,10 @@
       <c r="H17" s="2">
         <v>0</v>
       </c>
-      <c r="I17" s="6">
-        <v>1</v>
-      </c>
-      <c r="J17" s="11">
+      <c r="I17" s="4">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7">
         <v>0.41</v>
       </c>
       <c r="K17" s="2">
@@ -1766,7 +3490,7 @@
         <f t="shared" si="12"/>
         <v>104.55</v>
       </c>
-      <c r="T17" s="13" t="s">
+      <c r="T17" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1778,10 +3502,10 @@
       <c r="B18" s="2">
         <v>0</v>
       </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11">
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
         <v>0.4</v>
       </c>
       <c r="E18" s="2">
@@ -1799,10 +3523,10 @@
       <c r="H18" s="2">
         <v>0</v>
       </c>
-      <c r="I18" s="6">
-        <v>1</v>
-      </c>
-      <c r="J18" s="11">
+      <c r="I18" s="4">
+        <v>1</v>
+      </c>
+      <c r="J18" s="7">
         <v>0.41</v>
       </c>
       <c r="K18" s="2">
@@ -1841,7 +3565,7 @@
         <f t="shared" si="12"/>
         <v>104.55</v>
       </c>
-      <c r="T18" s="13" t="s">
+      <c r="T18" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1853,10 +3577,10 @@
       <c r="B19" s="2">
         <v>0</v>
       </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19" s="11">
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
         <v>0.4</v>
       </c>
       <c r="E19" s="2">
@@ -1874,10 +3598,10 @@
       <c r="H19" s="2">
         <v>0</v>
       </c>
-      <c r="I19" s="6">
-        <v>1</v>
-      </c>
-      <c r="J19" s="11">
+      <c r="I19" s="4">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7">
         <v>0.45</v>
       </c>
       <c r="K19" s="2">
@@ -1916,7 +3640,7 @@
         <f t="shared" si="12"/>
         <v>114.75</v>
       </c>
-      <c r="T19" s="13" t="s">
+      <c r="T19" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1928,10 +3652,10 @@
       <c r="B20" s="2">
         <v>0</v>
       </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20" s="11">
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
         <v>0.69</v>
       </c>
       <c r="E20" s="2">
@@ -1949,10 +3673,10 @@
       <c r="H20" s="2">
         <v>0</v>
       </c>
-      <c r="I20" s="6">
-        <v>1</v>
-      </c>
-      <c r="J20" s="11">
+      <c r="I20" s="4">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7">
         <v>0.49</v>
       </c>
       <c r="K20" s="2">
@@ -1991,7 +3715,7 @@
         <f t="shared" si="12"/>
         <v>124.95</v>
       </c>
-      <c r="T20" s="12" t="s">
+      <c r="T20" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2008,30 +3732,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>